<commit_message>
Add (and use) information on ExisUnits (based on LEGO_internal result)
Move slack-variables to other variables
</commit_message>
<xml_diff>
--- a/data/example/Power_ThermalGen.xlsx
+++ b/data/example/Power_ThermalGen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD9EE54-D343-4DE0-8213-FFD2C4C1BA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7C8935-8694-4455-A57B-0B4DA8052ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power ThermalGen" sheetId="105" r:id="rId1"/>
@@ -978,7 +978,7 @@
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="O55" sqref="O55"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,7 +1237,7 @@
       <c r="Q7" s="18">
         <v>0</v>
       </c>
-      <c r="R7" s="20"/>
+      <c r="R7" s="12"/>
       <c r="S7" s="21">
         <v>0</v>
       </c>
@@ -1316,7 +1316,7 @@
       <c r="Q8" s="18">
         <v>2000000</v>
       </c>
-      <c r="R8" s="20"/>
+      <c r="R8" s="12"/>
       <c r="S8" s="21">
         <v>1</v>
       </c>
@@ -1392,7 +1392,7 @@
       <c r="Q9" s="18">
         <v>2000000</v>
       </c>
-      <c r="R9" s="20"/>
+      <c r="R9" s="12"/>
       <c r="S9" s="21">
         <v>1</v>
       </c>
@@ -1468,7 +1468,7 @@
       <c r="Q10" s="18">
         <v>2000000</v>
       </c>
-      <c r="R10" s="20"/>
+      <c r="R10" s="12"/>
       <c r="S10" s="21">
         <v>1</v>
       </c>
@@ -1544,7 +1544,7 @@
       <c r="Q11" s="18">
         <v>2000000</v>
       </c>
-      <c r="R11" s="20"/>
+      <c r="R11" s="12"/>
       <c r="S11" s="21">
         <v>1</v>
       </c>
@@ -1620,7 +1620,7 @@
       <c r="Q12" s="18">
         <v>1000000</v>
       </c>
-      <c r="R12" s="20"/>
+      <c r="R12" s="12"/>
       <c r="S12" s="21">
         <v>1</v>
       </c>
@@ -1696,7 +1696,7 @@
       <c r="Q13" s="18">
         <v>1000000</v>
       </c>
-      <c r="R13" s="20"/>
+      <c r="R13" s="12"/>
       <c r="S13" s="21">
         <v>1</v>
       </c>
@@ -1771,7 +1771,7 @@
       <c r="Q14" s="18">
         <v>1000000</v>
       </c>
-      <c r="R14" s="20"/>
+      <c r="R14" s="12"/>
       <c r="S14" s="21">
         <v>1</v>
       </c>
@@ -1846,7 +1846,7 @@
       <c r="Q15" s="18">
         <v>1000000</v>
       </c>
-      <c r="R15" s="20"/>
+      <c r="R15" s="12"/>
       <c r="S15" s="21">
         <v>1</v>
       </c>
@@ -1921,7 +1921,7 @@
       <c r="Q16" s="18">
         <v>1000000</v>
       </c>
-      <c r="R16" s="20"/>
+      <c r="R16" s="12"/>
       <c r="S16" s="21">
         <v>1</v>
       </c>
@@ -1996,7 +1996,7 @@
       <c r="Q17" s="18">
         <v>1000000</v>
       </c>
-      <c r="R17" s="20"/>
+      <c r="R17" s="12"/>
       <c r="S17" s="21">
         <v>1</v>
       </c>
@@ -2071,7 +2071,7 @@
       <c r="Q18" s="18">
         <v>1000000</v>
       </c>
-      <c r="R18" s="20"/>
+      <c r="R18" s="12"/>
       <c r="S18" s="21">
         <v>1</v>
       </c>
@@ -2146,7 +2146,7 @@
       <c r="Q19" s="18">
         <v>1000000</v>
       </c>
-      <c r="R19" s="20"/>
+      <c r="R19" s="12"/>
       <c r="S19" s="21">
         <v>1</v>
       </c>
@@ -2221,7 +2221,7 @@
       <c r="Q20" s="18">
         <v>1000000</v>
       </c>
-      <c r="R20" s="20"/>
+      <c r="R20" s="12"/>
       <c r="S20" s="21">
         <v>1</v>
       </c>
@@ -2296,7 +2296,7 @@
       <c r="Q21" s="18">
         <v>0</v>
       </c>
-      <c r="R21" s="20"/>
+      <c r="R21" s="12"/>
       <c r="S21" s="21">
         <v>1</v>
       </c>
@@ -2371,7 +2371,7 @@
       <c r="Q22" s="18">
         <v>0</v>
       </c>
-      <c r="R22" s="20"/>
+      <c r="R22" s="12"/>
       <c r="S22" s="21">
         <v>1</v>
       </c>
@@ -2446,7 +2446,7 @@
       <c r="Q23" s="18">
         <v>0</v>
       </c>
-      <c r="R23" s="20"/>
+      <c r="R23" s="12"/>
       <c r="S23" s="21">
         <v>1</v>
       </c>
@@ -2521,7 +2521,7 @@
       <c r="Q24" s="18">
         <v>0</v>
       </c>
-      <c r="R24" s="20"/>
+      <c r="R24" s="12"/>
       <c r="S24" s="21">
         <v>1</v>
       </c>
@@ -2596,7 +2596,7 @@
       <c r="Q25" s="18">
         <v>0</v>
       </c>
-      <c r="R25" s="20"/>
+      <c r="R25" s="12"/>
       <c r="S25" s="21">
         <v>1</v>
       </c>
@@ -2671,7 +2671,7 @@
       <c r="Q26" s="18">
         <v>1000000</v>
       </c>
-      <c r="R26" s="20"/>
+      <c r="R26" s="12"/>
       <c r="S26" s="21">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Implement min up/down time for thermal generators
</commit_message>
<xml_diff>
--- a/data/example/Power_ThermalGen.xlsx
+++ b/data/example/Power_ThermalGen.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7C8935-8694-4455-A57B-0B4DA8052ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7600B457-275B-4429-B9F8-A1CEAFFE3537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power ThermalGen" sheetId="105" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Power ThermalGen'!$B$7:$W$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Power ThermalGen'!$B$7:$Y$26</definedName>
     <definedName name="businfo">#REF!</definedName>
     <definedName name="demand">#REF!</definedName>
     <definedName name="dsmdelaytime">#REF!</definedName>
@@ -39,7 +39,7 @@
     <definedName name="runofriver">#REF!</definedName>
     <definedName name="sCodeName">#REF!</definedName>
     <definedName name="storage">#REF!</definedName>
-    <definedName name="thermalgen">'Power ThermalGen'!$B$7:$W$26</definedName>
+    <definedName name="thermalgen">'Power ThermalGen'!$B$7:$Y$26</definedName>
     <definedName name="weight_k">#REF!</definedName>
     <definedName name="weight_rp">#REF!</definedName>
     <definedName name="zones">#REF!</definedName>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="73">
   <si>
     <t>[MW]</t>
   </si>
@@ -353,6 +353,15 @@
   </si>
   <si>
     <t>Import2</t>
+  </si>
+  <si>
+    <t>[h]</t>
+  </si>
+  <si>
+    <t>MinUpTime</t>
+  </si>
+  <si>
+    <t>MinDownTime</t>
   </si>
 </sst>
 </file>
@@ -973,12 +982,12 @@
   <sheetPr codeName="Tabelle2">
     <tabColor rgb="FF008080"/>
   </sheetPr>
-  <dimension ref="B1:AB48"/>
+  <dimension ref="B1:AD48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="O55" sqref="O55"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
+      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,18 +995,18 @@
     <col min="1" max="1" width="3" style="2" customWidth="1"/>
     <col min="2" max="2" width="34" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="23" width="12" style="2" customWidth="1"/>
-    <col min="24" max="24" width="16" style="2" customWidth="1"/>
-    <col min="25" max="26" width="14" style="2" customWidth="1"/>
-    <col min="27" max="16384" width="11.42578125" style="2"/>
+    <col min="4" max="25" width="12" style="2" customWidth="1"/>
+    <col min="26" max="26" width="16" style="2" customWidth="1"/>
+    <col min="27" max="28" width="14" style="2" customWidth="1"/>
+    <col min="29" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:30" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1017,64 +1026,70 @@
         <v>17</v>
       </c>
       <c r="J3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="R3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="S3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="T3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="U3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="V3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="W3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="X3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="W3" s="4" t="s">
+      <c r="Y3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="X3" s="26" t="s">
+      <c r="Z3" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="Y3" s="26" t="s">
+      <c r="AA3" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="Z3" s="26" t="s">
+      <c r="AB3" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="AA3" s="26" t="s">
+      <c r="AC3" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="AB3" s="26" t="s">
+      <c r="AD3" s="26" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
       <c r="E4" s="5"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -1094,13 +1109,15 @@
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
-      <c r="X4" s="27"/>
-      <c r="Y4" s="27"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
       <c r="Z4" s="27"/>
       <c r="AA4" s="27"/>
       <c r="AB4" s="27"/>
-    </row>
-    <row r="5" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AC4" s="27"/>
+      <c r="AD4" s="27"/>
+    </row>
+    <row r="5" spans="2:30" x14ac:dyDescent="0.25">
       <c r="E5" s="7"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -1120,13 +1137,15 @@
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
       <c r="W5" s="6"/>
-      <c r="X5" s="27"/>
-      <c r="Y5" s="27"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
       <c r="Z5" s="27"/>
       <c r="AA5" s="27"/>
       <c r="AB5" s="27"/>
-    </row>
-    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AC5" s="27"/>
+      <c r="AD5" s="27"/>
+    </row>
+    <row r="6" spans="2:30" x14ac:dyDescent="0.25">
       <c r="E6" s="8" t="s">
         <v>20</v>
       </c>
@@ -1143,52 +1162,58 @@
         <v>0</v>
       </c>
       <c r="J6" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="L6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="M6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="N6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="O6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="P6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="Q6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="R6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="Q6" s="8" t="s">
+      <c r="S6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="R6" s="8" t="s">
+      <c r="T6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="S6" s="8" t="s">
+      <c r="U6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="T6" s="8" t="s">
+      <c r="V6" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="U6" s="8" t="s">
+      <c r="W6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="V6" s="8" t="s">
+      <c r="X6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="W6" s="9"/>
-      <c r="X6" s="28"/>
-      <c r="Y6" s="28"/>
+      <c r="Y6" s="9"/>
       <c r="Z6" s="28"/>
       <c r="AA6" s="28"/>
       <c r="AB6" s="28"/>
-    </row>
-    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AC6" s="28"/>
+      <c r="AD6" s="28"/>
+    </row>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>30</v>
       </c>
@@ -1213,61 +1238,63 @@
       <c r="I7" s="14">
         <v>0</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14">
         <v>0</v>
       </c>
-      <c r="K7" s="14">
+      <c r="M7" s="14">
         <v>0</v>
       </c>
-      <c r="L7" s="15">
+      <c r="N7" s="15">
         <v>8</v>
       </c>
-      <c r="M7" s="16">
+      <c r="O7" s="16">
         <v>1</v>
       </c>
-      <c r="N7" s="17">
+      <c r="P7" s="17">
         <v>15</v>
-      </c>
-      <c r="O7" s="18">
-        <v>0</v>
-      </c>
-      <c r="P7" s="19">
-        <v>0</v>
       </c>
       <c r="Q7" s="18">
         <v>0</v>
       </c>
-      <c r="R7" s="12"/>
-      <c r="S7" s="21">
+      <c r="R7" s="19">
         <v>0</v>
       </c>
-      <c r="T7" s="20">
+      <c r="S7" s="18">
         <v>0</v>
       </c>
-      <c r="U7" s="20">
+      <c r="T7" s="12"/>
+      <c r="U7" s="21">
+        <v>0</v>
+      </c>
+      <c r="V7" s="20">
+        <v>0</v>
+      </c>
+      <c r="W7" s="20">
         <v>0.97</v>
       </c>
-      <c r="V7" s="22">
+      <c r="X7" s="22">
         <v>0</v>
       </c>
-      <c r="W7" s="23">
+      <c r="Y7" s="23">
         <v>15</v>
       </c>
-      <c r="X7" s="29" t="s">
+      <c r="Z7" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="Y7" s="30">
+      <c r="AA7" s="30">
         <v>2010</v>
       </c>
-      <c r="Z7" s="30"/>
-      <c r="AA7" s="31">
+      <c r="AB7" s="30"/>
+      <c r="AC7" s="31">
         <v>47.491300000000003</v>
       </c>
-      <c r="AB7" s="31">
+      <c r="AD7" s="31">
         <v>12.818199999999999</v>
       </c>
     </row>
-    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>31</v>
       </c>
@@ -1292,58 +1319,60 @@
       <c r="I8" s="14">
         <v>88.2</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14">
         <v>176.4</v>
       </c>
-      <c r="K8" s="14">
+      <c r="M8" s="14">
         <v>-176.4</v>
       </c>
-      <c r="L8" s="15">
+      <c r="N8" s="15">
         <v>6</v>
       </c>
-      <c r="M8" s="16">
+      <c r="O8" s="16">
         <v>0.02</v>
       </c>
-      <c r="N8" s="17">
+      <c r="P8" s="17">
         <v>2400</v>
       </c>
-      <c r="O8" s="18">
+      <c r="Q8" s="18">
         <v>50000</v>
       </c>
-      <c r="P8" s="19">
+      <c r="R8" s="19">
         <v>6</v>
       </c>
-      <c r="Q8" s="18">
+      <c r="S8" s="18">
         <v>2000000</v>
       </c>
-      <c r="R8" s="12"/>
-      <c r="S8" s="21">
+      <c r="T8" s="12"/>
+      <c r="U8" s="21">
         <v>1</v>
       </c>
-      <c r="T8" s="20">
+      <c r="V8" s="20">
         <v>145591.30710000001</v>
       </c>
-      <c r="U8" s="20">
+      <c r="W8" s="20">
         <v>0.95</v>
       </c>
-      <c r="V8" s="22">
+      <c r="X8" s="22">
         <v>0.35499999999999998</v>
       </c>
-      <c r="W8" s="23">
+      <c r="Y8" s="23">
         <v>49.700699999999998</v>
       </c>
-      <c r="X8" s="2" t="s">
+      <c r="Z8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="32">
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="32">
         <v>46.77</v>
       </c>
-      <c r="AB8" s="32">
+      <c r="AD8" s="32">
         <v>13.746700000000001</v>
       </c>
     </row>
-    <row r="9" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>32</v>
       </c>
@@ -1368,58 +1397,60 @@
       <c r="I9" s="14">
         <v>30.465</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14">
         <v>60.93</v>
       </c>
-      <c r="K9" s="14">
+      <c r="M9" s="14">
         <v>-60.93</v>
       </c>
-      <c r="L9" s="15">
+      <c r="N9" s="15">
         <v>6</v>
       </c>
-      <c r="M9" s="16">
+      <c r="O9" s="16">
         <v>2.0500000000000001E-2</v>
       </c>
-      <c r="N9" s="17">
+      <c r="P9" s="17">
         <v>2300</v>
       </c>
-      <c r="O9" s="18">
+      <c r="Q9" s="18">
         <v>50000</v>
       </c>
-      <c r="P9" s="19">
+      <c r="R9" s="19">
         <v>6.05</v>
       </c>
-      <c r="Q9" s="18">
+      <c r="S9" s="18">
         <v>2000000</v>
       </c>
-      <c r="R9" s="12"/>
-      <c r="S9" s="21">
+      <c r="T9" s="12"/>
+      <c r="U9" s="21">
         <v>1</v>
       </c>
-      <c r="T9" s="20">
+      <c r="V9" s="20">
         <v>146591.30710000001</v>
       </c>
-      <c r="U9" s="20">
+      <c r="W9" s="20">
         <v>0.95</v>
       </c>
-      <c r="V9" s="22">
+      <c r="X9" s="22">
         <v>0.33500000000000002</v>
       </c>
-      <c r="W9" s="23">
+      <c r="Y9" s="23">
         <v>50.923699999999997</v>
       </c>
-      <c r="X9" s="2" t="s">
+      <c r="Z9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="32">
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="32">
         <v>46.77</v>
       </c>
-      <c r="AB9" s="32">
+      <c r="AD9" s="32">
         <v>13.746700000000001</v>
       </c>
     </row>
-    <row r="10" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>33</v>
       </c>
@@ -1444,58 +1475,60 @@
       <c r="I10" s="14">
         <v>22.56</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14">
         <v>45.12</v>
       </c>
-      <c r="K10" s="14">
+      <c r="M10" s="14">
         <v>-45.12</v>
       </c>
-      <c r="L10" s="15">
+      <c r="N10" s="15">
         <v>6</v>
       </c>
-      <c r="M10" s="16">
+      <c r="O10" s="16">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="N10" s="17">
+      <c r="P10" s="17">
         <v>2300</v>
       </c>
-      <c r="O10" s="18">
+      <c r="Q10" s="18">
         <v>50000</v>
       </c>
-      <c r="P10" s="19">
+      <c r="R10" s="19">
         <v>6.1</v>
       </c>
-      <c r="Q10" s="18">
+      <c r="S10" s="18">
         <v>2000000</v>
       </c>
-      <c r="R10" s="12"/>
-      <c r="S10" s="21">
+      <c r="T10" s="12"/>
+      <c r="U10" s="21">
         <v>1</v>
       </c>
-      <c r="T10" s="20">
+      <c r="V10" s="20">
         <v>147591.30710000001</v>
       </c>
-      <c r="U10" s="20">
+      <c r="W10" s="20">
         <v>0.95</v>
       </c>
-      <c r="V10" s="22">
+      <c r="X10" s="22">
         <v>0.33200000000000002</v>
       </c>
-      <c r="W10" s="23">
+      <c r="Y10" s="23">
         <v>52.648899999999998</v>
       </c>
-      <c r="X10" s="2" t="s">
+      <c r="Z10" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="32">
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="32">
         <v>46.561055000000003</v>
       </c>
-      <c r="AB10" s="32">
+      <c r="AD10" s="32">
         <v>14.479570000000001</v>
       </c>
     </row>
-    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>34</v>
       </c>
@@ -1520,58 +1553,60 @@
       <c r="I11" s="14">
         <v>29.16</v>
       </c>
-      <c r="J11" s="14">
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14">
         <v>58.32</v>
       </c>
-      <c r="K11" s="14">
+      <c r="M11" s="14">
         <v>-58.32</v>
       </c>
-      <c r="L11" s="15">
+      <c r="N11" s="15">
         <v>6</v>
       </c>
-      <c r="M11" s="16">
+      <c r="O11" s="16">
         <v>2.1499999999999998E-2</v>
       </c>
-      <c r="N11" s="17">
+      <c r="P11" s="17">
         <v>2200</v>
       </c>
-      <c r="O11" s="18">
+      <c r="Q11" s="18">
         <v>50000</v>
       </c>
-      <c r="P11" s="19">
+      <c r="R11" s="19">
         <v>6.15</v>
       </c>
-      <c r="Q11" s="18">
+      <c r="S11" s="18">
         <v>2000000</v>
       </c>
-      <c r="R11" s="12"/>
-      <c r="S11" s="21">
+      <c r="T11" s="12"/>
+      <c r="U11" s="21">
         <v>1</v>
       </c>
-      <c r="T11" s="20">
+      <c r="V11" s="20">
         <v>148591.30710000001</v>
       </c>
-      <c r="U11" s="20">
+      <c r="W11" s="20">
         <v>0.95</v>
       </c>
-      <c r="V11" s="22">
+      <c r="X11" s="22">
         <v>0.31900000000000001</v>
       </c>
-      <c r="W11" s="23">
+      <c r="Y11" s="23">
         <v>49.143999999999998</v>
       </c>
-      <c r="X11" s="2" t="s">
+      <c r="Z11" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="Z11" s="3"/>
-      <c r="AA11" s="32">
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="32">
         <v>47.055199999999999</v>
       </c>
-      <c r="AB11" s="32">
+      <c r="AD11" s="32">
         <v>9.9000199999999996</v>
       </c>
     </row>
-    <row r="12" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>35</v>
       </c>
@@ -1596,58 +1631,60 @@
       <c r="I12" s="14">
         <v>200</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14">
         <v>200</v>
       </c>
-      <c r="K12" s="14">
+      <c r="M12" s="14">
         <v>-200</v>
       </c>
-      <c r="L12" s="15">
+      <c r="N12" s="15">
         <v>4</v>
       </c>
-      <c r="M12" s="16">
+      <c r="O12" s="16">
         <v>0.03</v>
       </c>
-      <c r="N12" s="17">
+      <c r="P12" s="17">
         <v>1800</v>
       </c>
-      <c r="O12" s="18">
+      <c r="Q12" s="18">
         <v>300000</v>
       </c>
-      <c r="P12" s="19">
+      <c r="R12" s="19">
         <v>3.8</v>
       </c>
-      <c r="Q12" s="18">
+      <c r="S12" s="18">
         <v>1000000</v>
       </c>
-      <c r="R12" s="12"/>
-      <c r="S12" s="21">
+      <c r="T12" s="12"/>
+      <c r="U12" s="21">
         <v>1</v>
       </c>
-      <c r="T12" s="20">
+      <c r="V12" s="20">
         <v>41818.779699999999</v>
       </c>
-      <c r="U12" s="20">
+      <c r="W12" s="20">
         <v>0.96</v>
       </c>
-      <c r="V12" s="22">
+      <c r="X12" s="22">
         <v>0.18099999999999999</v>
       </c>
-      <c r="W12" s="23">
+      <c r="Y12" s="23">
         <v>72</v>
       </c>
-      <c r="X12" s="2" t="s">
+      <c r="Z12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="Z12" s="3"/>
-      <c r="AA12" s="32">
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="32">
         <v>47.066462000000001</v>
       </c>
-      <c r="AB12" s="32">
+      <c r="AD12" s="32">
         <v>9.9157949999999992</v>
       </c>
     </row>
-    <row r="13" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>36</v>
       </c>
@@ -1672,57 +1709,59 @@
       <c r="I13" s="14">
         <v>100</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14">
         <v>200</v>
       </c>
-      <c r="K13" s="14">
+      <c r="M13" s="14">
         <v>-200</v>
       </c>
-      <c r="L13" s="15">
+      <c r="N13" s="15">
         <v>4</v>
       </c>
-      <c r="M13" s="16">
+      <c r="O13" s="16">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="N13" s="17">
+      <c r="P13" s="17">
         <v>1800</v>
       </c>
-      <c r="O13" s="18">
+      <c r="Q13" s="18">
         <v>300000</v>
       </c>
-      <c r="P13" s="19">
+      <c r="R13" s="19">
         <v>3.85</v>
       </c>
-      <c r="Q13" s="18">
+      <c r="S13" s="18">
         <v>1000000</v>
       </c>
-      <c r="R13" s="12"/>
-      <c r="S13" s="21">
+      <c r="T13" s="12"/>
+      <c r="U13" s="21">
         <v>1</v>
       </c>
-      <c r="T13" s="20">
+      <c r="V13" s="20">
         <v>42818.779699999999</v>
       </c>
-      <c r="U13" s="20">
+      <c r="W13" s="20">
         <v>0.96</v>
       </c>
-      <c r="V13" s="22">
+      <c r="X13" s="22">
         <v>0.18099999999999999</v>
       </c>
-      <c r="W13" s="23">
+      <c r="Y13" s="23">
         <v>72</v>
       </c>
-      <c r="X13" s="2" t="s">
+      <c r="Z13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AA13" s="31">
+      <c r="AC13" s="31">
         <v>47.491300000000003</v>
       </c>
-      <c r="AB13" s="31">
+      <c r="AD13" s="31">
         <v>12.818199999999999</v>
       </c>
     </row>
-    <row r="14" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>37</v>
       </c>
@@ -1747,57 +1786,59 @@
       <c r="I14" s="14">
         <v>100</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14">
         <v>200</v>
       </c>
-      <c r="K14" s="14">
+      <c r="M14" s="14">
         <v>-200</v>
       </c>
-      <c r="L14" s="15">
+      <c r="N14" s="15">
         <v>4</v>
       </c>
-      <c r="M14" s="16">
+      <c r="O14" s="16">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="N14" s="17">
+      <c r="P14" s="17">
         <v>1800</v>
       </c>
-      <c r="O14" s="18">
+      <c r="Q14" s="18">
         <v>300000</v>
       </c>
-      <c r="P14" s="19">
+      <c r="R14" s="19">
         <v>3.9</v>
       </c>
-      <c r="Q14" s="18">
+      <c r="S14" s="18">
         <v>1000000</v>
       </c>
-      <c r="R14" s="12"/>
-      <c r="S14" s="21">
+      <c r="T14" s="12"/>
+      <c r="U14" s="21">
         <v>1</v>
       </c>
-      <c r="T14" s="20">
+      <c r="V14" s="20">
         <v>43818.779699999999</v>
       </c>
-      <c r="U14" s="20">
+      <c r="W14" s="20">
         <v>0.96</v>
       </c>
-      <c r="V14" s="22">
+      <c r="X14" s="22">
         <v>0.18099999999999999</v>
       </c>
-      <c r="W14" s="23">
+      <c r="Y14" s="23">
         <v>72</v>
       </c>
-      <c r="X14" s="2" t="s">
+      <c r="Z14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AA14" s="32">
+      <c r="AC14" s="32">
         <v>46.77</v>
       </c>
-      <c r="AB14" s="32">
+      <c r="AD14" s="32">
         <v>13.746700000000001</v>
       </c>
     </row>
-    <row r="15" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
         <v>38</v>
       </c>
@@ -1822,57 +1863,59 @@
       <c r="I15" s="14">
         <v>100</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14">
         <v>200</v>
       </c>
-      <c r="K15" s="14">
+      <c r="M15" s="14">
         <v>-200</v>
       </c>
-      <c r="L15" s="15">
+      <c r="N15" s="15">
         <v>4</v>
       </c>
-      <c r="M15" s="16">
+      <c r="O15" s="16">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="N15" s="17">
+      <c r="P15" s="17">
         <v>1800</v>
       </c>
-      <c r="O15" s="18">
+      <c r="Q15" s="18">
         <v>300000</v>
       </c>
-      <c r="P15" s="19">
+      <c r="R15" s="19">
         <v>3.95</v>
       </c>
-      <c r="Q15" s="18">
+      <c r="S15" s="18">
         <v>1000000</v>
       </c>
-      <c r="R15" s="12"/>
-      <c r="S15" s="21">
+      <c r="T15" s="12"/>
+      <c r="U15" s="21">
         <v>1</v>
       </c>
-      <c r="T15" s="20">
+      <c r="V15" s="20">
         <v>44818.779699999999</v>
       </c>
-      <c r="U15" s="20">
+      <c r="W15" s="20">
         <v>0.96</v>
       </c>
-      <c r="V15" s="22">
+      <c r="X15" s="22">
         <v>0.18099999999999999</v>
       </c>
-      <c r="W15" s="23">
+      <c r="Y15" s="23">
         <v>72</v>
       </c>
-      <c r="X15" s="2" t="s">
+      <c r="Z15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AA15" s="32">
+      <c r="AC15" s="32">
         <v>46.77</v>
       </c>
-      <c r="AB15" s="32">
+      <c r="AD15" s="32">
         <v>13.746700000000001</v>
       </c>
     </row>
-    <row r="16" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
         <v>39</v>
       </c>
@@ -1897,57 +1940,59 @@
       <c r="I16" s="14">
         <v>100</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14">
         <v>200</v>
       </c>
-      <c r="K16" s="14">
+      <c r="M16" s="14">
         <v>-200</v>
       </c>
-      <c r="L16" s="15">
+      <c r="N16" s="15">
         <v>4</v>
       </c>
-      <c r="M16" s="16">
+      <c r="O16" s="16">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="N16" s="17">
+      <c r="P16" s="17">
         <v>1800</v>
       </c>
-      <c r="O16" s="18">
+      <c r="Q16" s="18">
         <v>300000</v>
       </c>
-      <c r="P16" s="19">
+      <c r="R16" s="19">
         <v>4</v>
       </c>
-      <c r="Q16" s="18">
+      <c r="S16" s="18">
         <v>1000000</v>
       </c>
-      <c r="R16" s="12"/>
-      <c r="S16" s="21">
+      <c r="T16" s="12"/>
+      <c r="U16" s="21">
         <v>1</v>
       </c>
-      <c r="T16" s="20">
+      <c r="V16" s="20">
         <v>45818.779699999999</v>
       </c>
-      <c r="U16" s="20">
+      <c r="W16" s="20">
         <v>0.96</v>
       </c>
-      <c r="V16" s="22">
+      <c r="X16" s="22">
         <v>0.18099999999999999</v>
       </c>
-      <c r="W16" s="23">
+      <c r="Y16" s="23">
         <v>72</v>
       </c>
-      <c r="X16" s="2" t="s">
+      <c r="Z16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AA16" s="32">
+      <c r="AC16" s="32">
         <v>46.561055000000003</v>
       </c>
-      <c r="AB16" s="32">
+      <c r="AD16" s="32">
         <v>14.479570000000001</v>
       </c>
     </row>
-    <row r="17" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>40</v>
       </c>
@@ -1972,57 +2017,59 @@
       <c r="I17" s="14">
         <v>100</v>
       </c>
-      <c r="J17" s="14">
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14">
         <v>200</v>
       </c>
-      <c r="K17" s="14">
+      <c r="M17" s="14">
         <v>-200</v>
       </c>
-      <c r="L17" s="15">
+      <c r="N17" s="15">
         <v>4</v>
       </c>
-      <c r="M17" s="16">
+      <c r="O17" s="16">
         <v>0.04</v>
       </c>
-      <c r="N17" s="17">
+      <c r="P17" s="17">
         <v>1800</v>
       </c>
-      <c r="O17" s="18">
+      <c r="Q17" s="18">
         <v>300000</v>
       </c>
-      <c r="P17" s="19">
+      <c r="R17" s="19">
         <v>4.05</v>
       </c>
-      <c r="Q17" s="18">
+      <c r="S17" s="18">
         <v>1000000</v>
       </c>
-      <c r="R17" s="12"/>
-      <c r="S17" s="21">
+      <c r="T17" s="12"/>
+      <c r="U17" s="21">
         <v>1</v>
       </c>
-      <c r="T17" s="20">
+      <c r="V17" s="20">
         <v>46818.779699999999</v>
       </c>
-      <c r="U17" s="20">
+      <c r="W17" s="20">
         <v>0.96</v>
       </c>
-      <c r="V17" s="22">
+      <c r="X17" s="22">
         <v>0.18099999999999999</v>
       </c>
-      <c r="W17" s="23">
+      <c r="Y17" s="23">
         <v>72</v>
       </c>
-      <c r="X17" s="2" t="s">
+      <c r="Z17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AA17" s="32">
+      <c r="AC17" s="32">
         <v>47.055199999999999</v>
       </c>
-      <c r="AB17" s="32">
+      <c r="AD17" s="32">
         <v>9.9000199999999996</v>
       </c>
     </row>
-    <row r="18" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
         <v>41</v>
       </c>
@@ -2047,57 +2094,59 @@
       <c r="I18" s="14">
         <v>100</v>
       </c>
-      <c r="J18" s="14">
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14">
         <v>200</v>
       </c>
-      <c r="K18" s="14">
+      <c r="M18" s="14">
         <v>-200</v>
       </c>
-      <c r="L18" s="15">
+      <c r="N18" s="15">
         <v>4</v>
       </c>
-      <c r="M18" s="16">
+      <c r="O18" s="16">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="N18" s="17">
+      <c r="P18" s="17">
         <v>1800</v>
       </c>
-      <c r="O18" s="18">
+      <c r="Q18" s="18">
         <v>300000</v>
       </c>
-      <c r="P18" s="19">
+      <c r="R18" s="19">
         <v>4.0999999999999996</v>
       </c>
-      <c r="Q18" s="18">
+      <c r="S18" s="18">
         <v>1000000</v>
       </c>
-      <c r="R18" s="12"/>
-      <c r="S18" s="21">
+      <c r="T18" s="12"/>
+      <c r="U18" s="21">
         <v>1</v>
       </c>
-      <c r="T18" s="20">
+      <c r="V18" s="20">
         <v>47818.779699999999</v>
       </c>
-      <c r="U18" s="20">
+      <c r="W18" s="20">
         <v>0.96</v>
       </c>
-      <c r="V18" s="22">
+      <c r="X18" s="22">
         <v>0.18099999999999999</v>
       </c>
-      <c r="W18" s="23">
+      <c r="Y18" s="23">
         <v>72</v>
       </c>
-      <c r="X18" s="2" t="s">
+      <c r="Z18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AA18" s="32">
+      <c r="AC18" s="32">
         <v>47.066462000000001</v>
       </c>
-      <c r="AB18" s="32">
+      <c r="AD18" s="32">
         <v>9.9157949999999992</v>
       </c>
     </row>
-    <row r="19" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
         <v>42</v>
       </c>
@@ -2122,57 +2171,59 @@
       <c r="I19" s="14">
         <v>100</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14">
         <v>200</v>
       </c>
-      <c r="K19" s="14">
+      <c r="M19" s="14">
         <v>-200</v>
       </c>
-      <c r="L19" s="15">
+      <c r="N19" s="15">
         <v>4</v>
       </c>
-      <c r="M19" s="16">
+      <c r="O19" s="16">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="N19" s="17">
+      <c r="P19" s="17">
         <v>1800</v>
       </c>
-      <c r="O19" s="18">
+      <c r="Q19" s="18">
         <v>300000</v>
       </c>
-      <c r="P19" s="19">
+      <c r="R19" s="19">
         <v>4.1500000000000004</v>
       </c>
-      <c r="Q19" s="18">
+      <c r="S19" s="18">
         <v>1000000</v>
       </c>
-      <c r="R19" s="12"/>
-      <c r="S19" s="21">
+      <c r="T19" s="12"/>
+      <c r="U19" s="21">
         <v>1</v>
       </c>
-      <c r="T19" s="20">
+      <c r="V19" s="20">
         <v>48818.779699999999</v>
       </c>
-      <c r="U19" s="20">
+      <c r="W19" s="20">
         <v>0.96</v>
       </c>
-      <c r="V19" s="22">
+      <c r="X19" s="22">
         <v>0.18099999999999999</v>
       </c>
-      <c r="W19" s="23">
+      <c r="Y19" s="23">
         <v>72</v>
       </c>
-      <c r="X19" s="2" t="s">
+      <c r="Z19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AA19" s="31">
+      <c r="AC19" s="31">
         <v>47.491300000000003</v>
       </c>
-      <c r="AB19" s="31">
+      <c r="AD19" s="31">
         <v>12.818199999999999</v>
       </c>
     </row>
-    <row r="20" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
         <v>43</v>
       </c>
@@ -2197,57 +2248,59 @@
       <c r="I20" s="14">
         <v>100</v>
       </c>
-      <c r="J20" s="14">
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14">
         <v>200</v>
       </c>
-      <c r="K20" s="14">
+      <c r="M20" s="14">
         <v>-200</v>
       </c>
-      <c r="L20" s="15">
+      <c r="N20" s="15">
         <v>4</v>
       </c>
-      <c r="M20" s="16">
+      <c r="O20" s="16">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="N20" s="17">
+      <c r="P20" s="17">
         <v>1800</v>
       </c>
-      <c r="O20" s="18">
+      <c r="Q20" s="18">
         <v>300000</v>
       </c>
-      <c r="P20" s="19">
+      <c r="R20" s="19">
         <v>4.2</v>
       </c>
-      <c r="Q20" s="18">
+      <c r="S20" s="18">
         <v>1000000</v>
       </c>
-      <c r="R20" s="12"/>
-      <c r="S20" s="21">
+      <c r="T20" s="12"/>
+      <c r="U20" s="21">
         <v>1</v>
       </c>
-      <c r="T20" s="20">
+      <c r="V20" s="20">
         <v>49818.779699999999</v>
       </c>
-      <c r="U20" s="20">
+      <c r="W20" s="20">
         <v>0.96</v>
       </c>
-      <c r="V20" s="22">
+      <c r="X20" s="22">
         <v>0.18099999999999999</v>
       </c>
-      <c r="W20" s="23">
+      <c r="Y20" s="23">
         <v>72</v>
       </c>
-      <c r="X20" s="2" t="s">
+      <c r="Z20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AA20" s="32">
+      <c r="AC20" s="32">
         <v>46.77</v>
       </c>
-      <c r="AB20" s="32">
+      <c r="AD20" s="32">
         <v>13.746700000000001</v>
       </c>
     </row>
-    <row r="21" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
         <v>44</v>
       </c>
@@ -2273,56 +2326,62 @@
         <v>360</v>
       </c>
       <c r="J21" s="14">
+        <v>3</v>
+      </c>
+      <c r="K21" s="14">
+        <v>2</v>
+      </c>
+      <c r="L21" s="14">
         <v>180</v>
       </c>
-      <c r="K21" s="14">
+      <c r="M21" s="14">
         <v>-180</v>
       </c>
-      <c r="L21" s="15">
+      <c r="N21" s="15">
         <v>2.5</v>
       </c>
-      <c r="M21" s="16">
+      <c r="O21" s="16">
         <v>3.0300000000000001E-2</v>
       </c>
-      <c r="N21" s="17">
+      <c r="P21" s="17">
         <v>2000</v>
       </c>
-      <c r="O21" s="18">
+      <c r="Q21" s="18">
         <v>100000</v>
       </c>
-      <c r="P21" s="19">
+      <c r="R21" s="19">
         <v>4.03</v>
       </c>
-      <c r="Q21" s="18">
+      <c r="S21" s="18">
         <v>0</v>
       </c>
-      <c r="R21" s="12"/>
-      <c r="S21" s="21">
+      <c r="T21" s="12"/>
+      <c r="U21" s="21">
         <v>1</v>
       </c>
-      <c r="T21" s="20">
+      <c r="V21" s="20">
         <v>24781.499100000001</v>
       </c>
-      <c r="U21" s="20">
+      <c r="W21" s="20">
         <v>0.96</v>
       </c>
-      <c r="V21" s="22">
+      <c r="X21" s="22">
         <v>0.18099999999999999</v>
       </c>
-      <c r="W21" s="23">
+      <c r="Y21" s="23">
         <v>67.5</v>
       </c>
-      <c r="X21" s="2" t="s">
+      <c r="Z21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AA21" s="32">
+      <c r="AC21" s="32">
         <v>46.77</v>
       </c>
-      <c r="AB21" s="32">
+      <c r="AD21" s="32">
         <v>13.746700000000001</v>
       </c>
     </row>
-    <row r="22" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
         <v>45</v>
       </c>
@@ -2348,56 +2407,60 @@
         <v>360</v>
       </c>
       <c r="J22" s="14">
+        <v>3</v>
+      </c>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14">
         <v>180</v>
       </c>
-      <c r="K22" s="14">
+      <c r="M22" s="14">
         <v>-180</v>
       </c>
-      <c r="L22" s="15">
+      <c r="N22" s="15">
         <v>2.5</v>
       </c>
-      <c r="M22" s="16">
+      <c r="O22" s="16">
         <v>3.0599999999999999E-2</v>
       </c>
-      <c r="N22" s="17">
+      <c r="P22" s="17">
         <v>2000</v>
       </c>
-      <c r="O22" s="18">
+      <c r="Q22" s="18">
         <v>100000</v>
       </c>
-      <c r="P22" s="19">
+      <c r="R22" s="19">
         <v>4.0599999999999996</v>
       </c>
-      <c r="Q22" s="18">
+      <c r="S22" s="18">
         <v>0</v>
       </c>
-      <c r="R22" s="12"/>
-      <c r="S22" s="21">
+      <c r="T22" s="12"/>
+      <c r="U22" s="21">
         <v>1</v>
       </c>
-      <c r="T22" s="20">
+      <c r="V22" s="20">
         <v>25781.499100000001</v>
       </c>
-      <c r="U22" s="20">
+      <c r="W22" s="20">
         <v>0.96</v>
       </c>
-      <c r="V22" s="22">
+      <c r="X22" s="22">
         <v>0.18099999999999999</v>
       </c>
-      <c r="W22" s="23">
+      <c r="Y22" s="23">
         <v>67.5</v>
       </c>
-      <c r="X22" s="2" t="s">
+      <c r="Z22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AA22" s="32">
+      <c r="AC22" s="32">
         <v>46.561055000000003</v>
       </c>
-      <c r="AB22" s="32">
+      <c r="AD22" s="32">
         <v>14.479570000000001</v>
       </c>
     </row>
-    <row r="23" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>46</v>
       </c>
@@ -2422,57 +2485,61 @@
       <c r="I23" s="14">
         <v>360</v>
       </c>
-      <c r="J23" s="14">
+      <c r="J23" s="14"/>
+      <c r="K23" s="14">
+        <v>4</v>
+      </c>
+      <c r="L23" s="14">
         <v>180</v>
       </c>
-      <c r="K23" s="14">
+      <c r="M23" s="14">
         <v>-180</v>
       </c>
-      <c r="L23" s="15">
+      <c r="N23" s="15">
         <v>2.5</v>
       </c>
-      <c r="M23" s="16">
+      <c r="O23" s="16">
         <v>3.09E-2</v>
       </c>
-      <c r="N23" s="17">
+      <c r="P23" s="17">
         <v>2000</v>
       </c>
-      <c r="O23" s="18">
+      <c r="Q23" s="18">
         <v>100000</v>
       </c>
-      <c r="P23" s="19">
+      <c r="R23" s="19">
         <v>4.09</v>
       </c>
-      <c r="Q23" s="18">
+      <c r="S23" s="18">
         <v>0</v>
       </c>
-      <c r="R23" s="12"/>
-      <c r="S23" s="21">
+      <c r="T23" s="12"/>
+      <c r="U23" s="21">
         <v>1</v>
       </c>
-      <c r="T23" s="20">
+      <c r="V23" s="20">
         <v>26781.499100000001</v>
       </c>
-      <c r="U23" s="20">
+      <c r="W23" s="20">
         <v>0.96</v>
       </c>
-      <c r="V23" s="22">
+      <c r="X23" s="22">
         <v>0.18099999999999999</v>
       </c>
-      <c r="W23" s="23">
+      <c r="Y23" s="23">
         <v>67.5</v>
       </c>
-      <c r="X23" s="2" t="s">
+      <c r="Z23" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AA23" s="32">
+      <c r="AC23" s="32">
         <v>47.055199999999999</v>
       </c>
-      <c r="AB23" s="32">
+      <c r="AD23" s="32">
         <v>9.9000199999999996</v>
       </c>
     </row>
-    <row r="24" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
         <v>47</v>
       </c>
@@ -2497,57 +2564,59 @@
       <c r="I24" s="14">
         <v>360</v>
       </c>
-      <c r="J24" s="14">
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14">
         <v>180</v>
       </c>
-      <c r="K24" s="14">
+      <c r="M24" s="14">
         <v>-180</v>
       </c>
-      <c r="L24" s="15">
+      <c r="N24" s="15">
         <v>2.5</v>
       </c>
-      <c r="M24" s="16">
+      <c r="O24" s="16">
         <v>3.1199999999999999E-2</v>
       </c>
-      <c r="N24" s="17">
+      <c r="P24" s="17">
         <v>2000</v>
       </c>
-      <c r="O24" s="18">
+      <c r="Q24" s="18">
         <v>100000</v>
       </c>
-      <c r="P24" s="19">
+      <c r="R24" s="19">
         <v>4.12</v>
       </c>
-      <c r="Q24" s="18">
+      <c r="S24" s="18">
         <v>0</v>
       </c>
-      <c r="R24" s="12"/>
-      <c r="S24" s="21">
+      <c r="T24" s="12"/>
+      <c r="U24" s="21">
         <v>1</v>
       </c>
-      <c r="T24" s="20">
+      <c r="V24" s="20">
         <v>27781.499100000001</v>
       </c>
-      <c r="U24" s="20">
+      <c r="W24" s="20">
         <v>0.96</v>
       </c>
-      <c r="V24" s="22">
+      <c r="X24" s="22">
         <v>0.18099999999999999</v>
       </c>
-      <c r="W24" s="23">
+      <c r="Y24" s="23">
         <v>67.5</v>
       </c>
-      <c r="X24" s="2" t="s">
+      <c r="Z24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AA24" s="32">
+      <c r="AC24" s="32">
         <v>47.066462000000001</v>
       </c>
-      <c r="AB24" s="32">
+      <c r="AD24" s="32">
         <v>9.9157949999999992</v>
       </c>
     </row>
-    <row r="25" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>48</v>
       </c>
@@ -2573,56 +2642,62 @@
         <v>360</v>
       </c>
       <c r="J25" s="14">
+        <v>3</v>
+      </c>
+      <c r="K25" s="14">
+        <v>2</v>
+      </c>
+      <c r="L25" s="14">
         <v>180</v>
       </c>
-      <c r="K25" s="14">
+      <c r="M25" s="14">
         <v>-180</v>
       </c>
-      <c r="L25" s="15">
+      <c r="N25" s="15">
         <v>2.5</v>
       </c>
-      <c r="M25" s="16">
+      <c r="O25" s="16">
         <v>3.15E-2</v>
       </c>
-      <c r="N25" s="17">
+      <c r="P25" s="17">
         <v>2000</v>
       </c>
-      <c r="O25" s="18">
+      <c r="Q25" s="18">
         <v>100000</v>
       </c>
-      <c r="P25" s="19">
+      <c r="R25" s="19">
         <v>4.1500000000000004</v>
       </c>
-      <c r="Q25" s="18">
+      <c r="S25" s="18">
         <v>0</v>
       </c>
-      <c r="R25" s="12"/>
-      <c r="S25" s="21">
+      <c r="T25" s="12"/>
+      <c r="U25" s="21">
         <v>1</v>
       </c>
-      <c r="T25" s="20">
+      <c r="V25" s="20">
         <v>28781.499100000001</v>
       </c>
-      <c r="U25" s="20">
+      <c r="W25" s="20">
         <v>0.96</v>
       </c>
-      <c r="V25" s="22">
+      <c r="X25" s="22">
         <v>0.18099999999999999</v>
       </c>
-      <c r="W25" s="23">
+      <c r="Y25" s="23">
         <v>67.5</v>
       </c>
-      <c r="X25" s="2" t="s">
+      <c r="Z25" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AA25" s="31">
+      <c r="AC25" s="31">
         <v>47.491300000000003</v>
       </c>
-      <c r="AB25" s="31">
+      <c r="AD25" s="31">
         <v>12.818199999999999</v>
       </c>
     </row>
-    <row r="26" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
         <v>49</v>
       </c>
@@ -2647,61 +2722,63 @@
       <c r="I26" s="14">
         <v>397.62</v>
       </c>
-      <c r="J26" s="14">
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14">
         <v>198.81</v>
       </c>
-      <c r="K26" s="14">
+      <c r="M26" s="14">
         <v>-198.81</v>
       </c>
-      <c r="L26" s="15">
+      <c r="N26" s="15">
         <v>2.5</v>
       </c>
-      <c r="M26" s="16">
+      <c r="O26" s="16">
         <v>0.06</v>
       </c>
-      <c r="N26" s="17">
+      <c r="P26" s="17">
         <v>2000</v>
       </c>
-      <c r="O26" s="18">
+      <c r="Q26" s="18">
         <v>300000</v>
       </c>
-      <c r="P26" s="19">
+      <c r="R26" s="19">
         <v>3</v>
       </c>
-      <c r="Q26" s="18">
+      <c r="S26" s="18">
         <v>1000000</v>
       </c>
-      <c r="R26" s="12"/>
-      <c r="S26" s="21">
+      <c r="T26" s="12"/>
+      <c r="U26" s="21">
         <v>1</v>
       </c>
-      <c r="T26" s="20">
+      <c r="V26" s="20">
         <v>43367.623399999997</v>
       </c>
-      <c r="U26" s="20">
+      <c r="W26" s="20">
         <v>0.95</v>
       </c>
-      <c r="V26" s="22">
+      <c r="X26" s="22">
         <v>0.254</v>
       </c>
-      <c r="W26" s="23">
+      <c r="Y26" s="23">
         <v>160.7424</v>
       </c>
-      <c r="X26" s="2" t="s">
+      <c r="Z26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AA26" s="32">
+      <c r="AC26" s="32">
         <v>46.77</v>
       </c>
-      <c r="AB26" s="32">
+      <c r="AD26" s="32">
         <v>13.746700000000001</v>
       </c>
     </row>
-    <row r="27" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="AA27" s="32"/>
-      <c r="AB27" s="32"/>
-    </row>
-    <row r="28" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AC27" s="32"/>
+      <c r="AD27" s="32"/>
+    </row>
+    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
       <c r="D28" s="24"/>
       <c r="E28" s="24"/>
       <c r="F28" s="24"/>
@@ -2721,10 +2798,12 @@
       <c r="T28" s="24"/>
       <c r="U28" s="24"/>
       <c r="V28" s="24"/>
-      <c r="AA28" s="32"/>
-      <c r="AB28" s="32"/>
-    </row>
-    <row r="29" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="W28" s="24"/>
+      <c r="X28" s="24"/>
+      <c r="AC28" s="32"/>
+      <c r="AD28" s="32"/>
+    </row>
+    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
       <c r="D29" s="24"/>
       <c r="E29" s="24"/>
       <c r="F29" s="24"/>
@@ -2744,10 +2823,12 @@
       <c r="T29" s="24"/>
       <c r="U29" s="24"/>
       <c r="V29" s="24"/>
-      <c r="AA29" s="32"/>
-      <c r="AB29" s="32"/>
-    </row>
-    <row r="30" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="W29" s="24"/>
+      <c r="X29" s="24"/>
+      <c r="AC29" s="32"/>
+      <c r="AD29" s="32"/>
+    </row>
+    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
       <c r="D30" s="24"/>
       <c r="E30" s="24"/>
       <c r="F30" s="24"/>
@@ -2767,10 +2848,12 @@
       <c r="T30" s="24"/>
       <c r="U30" s="24"/>
       <c r="V30" s="24"/>
-      <c r="AA30" s="32"/>
-      <c r="AB30" s="32"/>
-    </row>
-    <row r="31" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="W30" s="24"/>
+      <c r="X30" s="24"/>
+      <c r="AC30" s="32"/>
+      <c r="AD30" s="32"/>
+    </row>
+    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
@@ -2790,8 +2873,10 @@
       <c r="T31" s="24"/>
       <c r="U31" s="24"/>
       <c r="V31" s="24"/>
-    </row>
-    <row r="32" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="W31" s="24"/>
+      <c r="X31" s="24"/>
+    </row>
+    <row r="32" spans="2:30" x14ac:dyDescent="0.25">
       <c r="D32" s="24"/>
       <c r="E32" s="24"/>
       <c r="F32" s="24"/>
@@ -2811,8 +2896,10 @@
       <c r="T32" s="24"/>
       <c r="U32" s="24"/>
       <c r="V32" s="24"/>
-    </row>
-    <row r="33" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="W32" s="24"/>
+      <c r="X32" s="24"/>
+    </row>
+    <row r="33" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D33" s="24"/>
       <c r="E33" s="24"/>
       <c r="F33" s="24"/>
@@ -2832,8 +2919,10 @@
       <c r="T33" s="24"/>
       <c r="U33" s="24"/>
       <c r="V33" s="24"/>
-    </row>
-    <row r="34" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="W33" s="24"/>
+      <c r="X33" s="24"/>
+    </row>
+    <row r="34" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D34" s="24"/>
       <c r="E34" s="24"/>
       <c r="F34" s="24"/>
@@ -2853,8 +2942,10 @@
       <c r="T34" s="24"/>
       <c r="U34" s="24"/>
       <c r="V34" s="24"/>
-    </row>
-    <row r="35" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="W34" s="24"/>
+      <c r="X34" s="24"/>
+    </row>
+    <row r="35" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D35" s="24"/>
       <c r="E35" s="24"/>
       <c r="F35" s="24"/>
@@ -2874,8 +2965,10 @@
       <c r="T35" s="24"/>
       <c r="U35" s="24"/>
       <c r="V35" s="24"/>
-    </row>
-    <row r="36" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="W35" s="24"/>
+      <c r="X35" s="24"/>
+    </row>
+    <row r="36" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D36" s="24"/>
       <c r="E36" s="24"/>
       <c r="F36" s="24"/>
@@ -2895,8 +2988,10 @@
       <c r="T36" s="24"/>
       <c r="U36" s="24"/>
       <c r="V36" s="24"/>
-    </row>
-    <row r="37" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="W36" s="24"/>
+      <c r="X36" s="24"/>
+    </row>
+    <row r="37" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D37" s="24"/>
       <c r="E37" s="24"/>
       <c r="F37" s="24"/>
@@ -2916,8 +3011,10 @@
       <c r="T37" s="24"/>
       <c r="U37" s="24"/>
       <c r="V37" s="24"/>
-    </row>
-    <row r="38" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="W37" s="24"/>
+      <c r="X37" s="24"/>
+    </row>
+    <row r="38" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D38" s="24"/>
       <c r="E38" s="24"/>
       <c r="F38" s="24"/>
@@ -2937,8 +3034,10 @@
       <c r="T38" s="24"/>
       <c r="U38" s="24"/>
       <c r="V38" s="24"/>
-    </row>
-    <row r="39" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="W38" s="24"/>
+      <c r="X38" s="24"/>
+    </row>
+    <row r="39" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D39" s="24"/>
       <c r="E39" s="24"/>
       <c r="F39" s="24"/>
@@ -2958,8 +3057,10 @@
       <c r="T39" s="24"/>
       <c r="U39" s="24"/>
       <c r="V39" s="24"/>
-    </row>
-    <row r="40" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="W39" s="24"/>
+      <c r="X39" s="24"/>
+    </row>
+    <row r="40" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D40" s="24"/>
       <c r="E40" s="24"/>
       <c r="F40" s="24"/>
@@ -2979,8 +3080,10 @@
       <c r="T40" s="24"/>
       <c r="U40" s="24"/>
       <c r="V40" s="24"/>
-    </row>
-    <row r="41" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="W40" s="24"/>
+      <c r="X40" s="24"/>
+    </row>
+    <row r="41" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D41" s="24"/>
       <c r="E41" s="24"/>
       <c r="F41" s="24"/>
@@ -3000,8 +3103,10 @@
       <c r="T41" s="24"/>
       <c r="U41" s="24"/>
       <c r="V41" s="24"/>
-    </row>
-    <row r="42" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="W41" s="24"/>
+      <c r="X41" s="24"/>
+    </row>
+    <row r="42" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D42" s="24"/>
       <c r="E42" s="24"/>
       <c r="F42" s="24"/>
@@ -3021,8 +3126,10 @@
       <c r="T42" s="24"/>
       <c r="U42" s="24"/>
       <c r="V42" s="24"/>
-    </row>
-    <row r="43" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="W42" s="24"/>
+      <c r="X42" s="24"/>
+    </row>
+    <row r="43" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D43" s="24"/>
       <c r="E43" s="24"/>
       <c r="F43" s="24"/>
@@ -3042,8 +3149,10 @@
       <c r="T43" s="24"/>
       <c r="U43" s="24"/>
       <c r="V43" s="24"/>
-    </row>
-    <row r="44" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="W43" s="24"/>
+      <c r="X43" s="24"/>
+    </row>
+    <row r="44" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D44" s="24"/>
       <c r="E44" s="24"/>
       <c r="F44" s="24"/>
@@ -3063,8 +3172,10 @@
       <c r="T44" s="24"/>
       <c r="U44" s="24"/>
       <c r="V44" s="24"/>
-    </row>
-    <row r="45" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="W44" s="24"/>
+      <c r="X44" s="24"/>
+    </row>
+    <row r="45" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D45" s="24"/>
       <c r="E45" s="24"/>
       <c r="F45" s="24"/>
@@ -3084,8 +3195,10 @@
       <c r="T45" s="24"/>
       <c r="U45" s="24"/>
       <c r="V45" s="24"/>
-    </row>
-    <row r="46" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="W45" s="24"/>
+      <c r="X45" s="24"/>
+    </row>
+    <row r="46" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D46" s="24"/>
       <c r="E46" s="24"/>
       <c r="F46" s="24"/>
@@ -3105,8 +3218,10 @@
       <c r="T46" s="24"/>
       <c r="U46" s="24"/>
       <c r="V46" s="24"/>
-    </row>
-    <row r="47" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="W46" s="24"/>
+      <c r="X46" s="24"/>
+    </row>
+    <row r="47" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D47" s="24"/>
       <c r="E47" s="24"/>
       <c r="F47" s="24"/>
@@ -3126,8 +3241,10 @@
       <c r="T47" s="24"/>
       <c r="U47" s="24"/>
       <c r="V47" s="24"/>
-    </row>
-    <row r="48" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="W47" s="24"/>
+      <c r="X47" s="24"/>
+    </row>
+    <row r="48" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D48" s="24"/>
       <c r="E48" s="24"/>
       <c r="F48" s="24"/>
@@ -3147,6 +3264,8 @@
       <c r="T48" s="24"/>
       <c r="U48" s="24"/>
       <c r="V48" s="24"/>
+      <c r="W48" s="24"/>
+      <c r="X48" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3156,6 +3275,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -3301,35 +3435,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3351,9 +3460,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Implement generation expansion for thermal units
Adjust indices order of some elements to have rp, k in front for power and storage
Adjust read-in of Power_ThermalGen
Set one CCGT EnableInvest to 1
</commit_message>
<xml_diff>
--- a/data/example/Power_ThermalGen.xlsx
+++ b/data/example/Power_ThermalGen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73388F8B-B25D-4736-AD9B-65A53FD30E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0156137F-A7E4-4888-AA2C-C4A199317592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power ThermalGen" sheetId="105" r:id="rId1"/>
@@ -984,10 +984,10 @@
   </sheetPr>
   <dimension ref="B1:AD48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="O55" sqref="O55"/>
-      <selection pane="bottomLeft" activeCell="U8" sqref="U8:U26"/>
+      <selection pane="bottomLeft" activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="T12" s="12"/>
       <c r="U12" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V12" s="20">
         <v>41818.779699999999</v>
@@ -3275,18 +3275,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3436,6 +3436,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -3447,14 +3455,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Re-implement Min Up-/Down-Time to be cyclic
Fill MinUp-/DownTime for Power_ThermalGen
</commit_message>
<xml_diff>
--- a/data/example/Power_ThermalGen.xlsx
+++ b/data/example/Power_ThermalGen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0156137F-A7E4-4888-AA2C-C4A199317592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CB1EAC-C24A-4C28-A5D9-D1F410FA6C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power ThermalGen" sheetId="105" r:id="rId1"/>
@@ -569,7 +569,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -652,6 +652,9 @@
     </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -984,10 +987,10 @@
   </sheetPr>
   <dimension ref="B1:AD48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="O55" sqref="O55"/>
-      <selection pane="bottomLeft" activeCell="U13" sqref="U13"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,8 +1241,12 @@
       <c r="I7" s="14">
         <v>0</v>
       </c>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
+      <c r="J7" s="33">
+        <v>1</v>
+      </c>
+      <c r="K7" s="33">
+        <v>1</v>
+      </c>
       <c r="L7" s="14">
         <v>0</v>
       </c>
@@ -1319,8 +1326,12 @@
       <c r="I8" s="14">
         <v>88.2</v>
       </c>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
+      <c r="J8" s="33">
+        <v>1</v>
+      </c>
+      <c r="K8" s="33">
+        <v>1</v>
+      </c>
       <c r="L8" s="14">
         <v>176.4</v>
       </c>
@@ -1397,8 +1408,12 @@
       <c r="I9" s="14">
         <v>30.465</v>
       </c>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
+      <c r="J9" s="33">
+        <v>1</v>
+      </c>
+      <c r="K9" s="33">
+        <v>1</v>
+      </c>
       <c r="L9" s="14">
         <v>60.93</v>
       </c>
@@ -1475,8 +1490,12 @@
       <c r="I10" s="14">
         <v>22.56</v>
       </c>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
+      <c r="J10" s="33">
+        <v>1</v>
+      </c>
+      <c r="K10" s="33">
+        <v>1</v>
+      </c>
       <c r="L10" s="14">
         <v>45.12</v>
       </c>
@@ -1553,8 +1572,12 @@
       <c r="I11" s="14">
         <v>29.16</v>
       </c>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
+      <c r="J11" s="33">
+        <v>1</v>
+      </c>
+      <c r="K11" s="33">
+        <v>1</v>
+      </c>
       <c r="L11" s="14">
         <v>58.32</v>
       </c>
@@ -1631,8 +1654,12 @@
       <c r="I12" s="14">
         <v>200</v>
       </c>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
+      <c r="J12" s="33">
+        <v>1</v>
+      </c>
+      <c r="K12" s="33">
+        <v>1</v>
+      </c>
       <c r="L12" s="14">
         <v>200</v>
       </c>
@@ -1709,8 +1736,12 @@
       <c r="I13" s="14">
         <v>100</v>
       </c>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
+      <c r="J13" s="33">
+        <v>1</v>
+      </c>
+      <c r="K13" s="33">
+        <v>1</v>
+      </c>
       <c r="L13" s="14">
         <v>200</v>
       </c>
@@ -1786,8 +1817,12 @@
       <c r="I14" s="14">
         <v>100</v>
       </c>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
+      <c r="J14" s="33">
+        <v>1</v>
+      </c>
+      <c r="K14" s="33">
+        <v>1</v>
+      </c>
       <c r="L14" s="14">
         <v>200</v>
       </c>
@@ -1863,8 +1898,12 @@
       <c r="I15" s="14">
         <v>100</v>
       </c>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
+      <c r="J15" s="33">
+        <v>1</v>
+      </c>
+      <c r="K15" s="33">
+        <v>1</v>
+      </c>
       <c r="L15" s="14">
         <v>200</v>
       </c>
@@ -1940,8 +1979,12 @@
       <c r="I16" s="14">
         <v>100</v>
       </c>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
+      <c r="J16" s="33">
+        <v>1</v>
+      </c>
+      <c r="K16" s="33">
+        <v>1</v>
+      </c>
       <c r="L16" s="14">
         <v>200</v>
       </c>
@@ -2017,8 +2060,12 @@
       <c r="I17" s="14">
         <v>100</v>
       </c>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
+      <c r="J17" s="33">
+        <v>1</v>
+      </c>
+      <c r="K17" s="33">
+        <v>1</v>
+      </c>
       <c r="L17" s="14">
         <v>200</v>
       </c>
@@ -2094,8 +2141,12 @@
       <c r="I18" s="14">
         <v>100</v>
       </c>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
+      <c r="J18" s="33">
+        <v>1</v>
+      </c>
+      <c r="K18" s="33">
+        <v>1</v>
+      </c>
       <c r="L18" s="14">
         <v>200</v>
       </c>
@@ -2171,8 +2222,12 @@
       <c r="I19" s="14">
         <v>100</v>
       </c>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
+      <c r="J19" s="33">
+        <v>1</v>
+      </c>
+      <c r="K19" s="33">
+        <v>1</v>
+      </c>
       <c r="L19" s="14">
         <v>200</v>
       </c>
@@ -2248,8 +2303,12 @@
       <c r="I20" s="14">
         <v>100</v>
       </c>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
+      <c r="J20" s="33">
+        <v>1</v>
+      </c>
+      <c r="K20" s="33">
+        <v>1</v>
+      </c>
       <c r="L20" s="14">
         <v>200</v>
       </c>
@@ -2325,10 +2384,10 @@
       <c r="I21" s="14">
         <v>360</v>
       </c>
-      <c r="J21" s="14">
+      <c r="J21" s="33">
         <v>3</v>
       </c>
-      <c r="K21" s="14">
+      <c r="K21" s="33">
         <v>2</v>
       </c>
       <c r="L21" s="14">
@@ -2406,10 +2465,12 @@
       <c r="I22" s="14">
         <v>360</v>
       </c>
-      <c r="J22" s="14">
+      <c r="J22" s="33">
         <v>3</v>
       </c>
-      <c r="K22" s="14"/>
+      <c r="K22" s="33">
+        <v>1</v>
+      </c>
       <c r="L22" s="14">
         <v>180</v>
       </c>
@@ -2485,8 +2546,10 @@
       <c r="I23" s="14">
         <v>360</v>
       </c>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14">
+      <c r="J23" s="33">
+        <v>1</v>
+      </c>
+      <c r="K23" s="33">
         <v>4</v>
       </c>
       <c r="L23" s="14">
@@ -2564,8 +2627,12 @@
       <c r="I24" s="14">
         <v>360</v>
       </c>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
+      <c r="J24" s="33">
+        <v>1</v>
+      </c>
+      <c r="K24" s="33">
+        <v>1</v>
+      </c>
       <c r="L24" s="14">
         <v>180</v>
       </c>
@@ -2641,10 +2708,10 @@
       <c r="I25" s="14">
         <v>360</v>
       </c>
-      <c r="J25" s="14">
+      <c r="J25" s="33">
         <v>3</v>
       </c>
-      <c r="K25" s="14">
+      <c r="K25" s="33">
         <v>2</v>
       </c>
       <c r="L25" s="14">
@@ -2722,8 +2789,12 @@
       <c r="I26" s="14">
         <v>397.62</v>
       </c>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
+      <c r="J26" s="33">
+        <v>1</v>
+      </c>
+      <c r="K26" s="33">
+        <v>1</v>
+      </c>
       <c r="L26" s="14">
         <v>198.81</v>
       </c>
@@ -3275,21 +3346,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -3435,10 +3491,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3460,19 +3541,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Implement eUCMaxOut2 & eUCMinOut, add vRes to MaxOut1 & 2
Add more variability to ThermalGen input (have more enableInvest, also for already existing units
</commit_message>
<xml_diff>
--- a/data/example/Power_ThermalGen.xlsx
+++ b/data/example/Power_ThermalGen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CB1EAC-C24A-4C28-A5D9-D1F410FA6C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC77ECE-8593-48FD-B765-89B86ABB3D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2451,7 +2451,7 @@
         <v>58</v>
       </c>
       <c r="E22" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" s="13">
         <v>400</v>
@@ -2578,7 +2578,7 @@
       </c>
       <c r="T23" s="12"/>
       <c r="U23" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V23" s="20">
         <v>26781.499100000001</v>
@@ -2659,7 +2659,7 @@
       </c>
       <c r="T24" s="12"/>
       <c r="U24" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V24" s="20">
         <v>27781.499100000001</v>

</xml_diff>

<commit_message>
Skip minUp/DownTime if it is set to 1
Adjust example for transition to have minUp/DownTime of 1 for all
</commit_message>
<xml_diff>
--- a/data/example/Power_ThermalGen.xlsx
+++ b/data/example/Power_ThermalGen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26084F25-EDB1-4D53-AC15-FE10E13DA022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34B48AB-5FE0-4079-91D3-FC97D4B0575A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioA" sheetId="105" r:id="rId1"/>
@@ -2894,10 +2894,10 @@
         <v>360</v>
       </c>
       <c r="K22" s="20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L22" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M22" s="19">
         <v>180</v>
@@ -2983,7 +2983,7 @@
         <v>360</v>
       </c>
       <c r="K23" s="20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L23" s="20">
         <v>1</v>
@@ -3075,7 +3075,7 @@
         <v>1</v>
       </c>
       <c r="L24" s="20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M24" s="19">
         <v>180</v>
@@ -3250,10 +3250,10 @@
         <v>360</v>
       </c>
       <c r="K26" s="20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L26" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M26" s="19">
         <v>180</v>
@@ -3501,9 +3501,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3653,26 +3656,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3696,9 +3688,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adjust Power_ThermalGen to v0.0.4r
</commit_message>
<xml_diff>
--- a/data/example/Power_ThermalGen.xlsx
+++ b/data/example/Power_ThermalGen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34B48AB-5FE0-4079-91D3-FC97D4B0575A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF9FCE0-7606-4DDC-8952-FF8B00CA0F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioA" sheetId="105" r:id="rId1"/>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="128">
   <si>
     <t>[MW]</t>
   </si>
@@ -520,7 +520,16 @@
     <t>Equivalent forced outage rate of the generator</t>
   </si>
   <si>
-    <t>v0.0.3</t>
+    <t>excl</t>
+  </si>
+  <si>
+    <t>v0.0.4r</t>
+  </si>
+  <si>
+    <t>Commission Year</t>
+  </si>
+  <si>
+    <t>Decommision Year</t>
   </si>
 </sst>
 </file>
@@ -1146,7 +1155,7 @@
         <v>88</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -1226,16 +1235,16 @@
         <v>19</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>52</v>
+        <v>126</v>
       </c>
       <c r="AA3" s="6" t="s">
-        <v>53</v>
+        <v>127</v>
       </c>
       <c r="AB3" s="6" t="s">
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="AC3" s="6" t="s">
-        <v>55</v>
+        <v>120</v>
       </c>
       <c r="AD3" s="6" t="s">
         <v>78</v>
@@ -1246,7 +1255,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>59</v>
+        <v>124</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>61</v>
@@ -3501,12 +3510,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3656,15 +3662,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3688,17 +3705,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>